<commit_message>
Login and Games search automation
</commit_message>
<xml_diff>
--- a/SteamGameFinder/Config.xlsx
+++ b/SteamGameFinder/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C2C312-72D2-4107-8A42-3E713100E89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1992" windowHeight="1140"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,19 +31,19 @@
     <t>https://store.steampowered.com/</t>
   </si>
   <si>
-    <t>D:\acte_facultate\an3\sem1\rpa\Proiect\Steam-game-finder\SteamGameFinder\games_to_find1.xlsx</t>
-  </si>
-  <si>
     <t>GameExcelPath</t>
   </si>
   <si>
     <t>SteamURL</t>
+  </si>
+  <si>
+    <t>C:\Users\david\Desktop\RPA\proiect\Steam-game-finder\SteamGameFinder\games_to_find1.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,27 +347,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="84.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,17 +375,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>

</xml_diff>